<commit_message>
Add household load profile in dataset
</commit_message>
<xml_diff>
--- a/data_in/data_structure.xlsx
+++ b/data_in/data_structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riw\Documents\repositories\pomato_data\data_in\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cw\repositories\PomatoData\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59BD49F-B238-4106-B41D-1414D5C50399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7575FEDD-35AD-4B4A-B1C1-A7427BFAA05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-108" windowWidth="40548" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="103">
   <si>
     <t xml:space="preserve">Attribute </t>
   </si>
@@ -332,6 +332,9 @@
   </si>
   <si>
     <t>storage_level</t>
+  </si>
+  <si>
+    <t>household_demand_el</t>
   </si>
 </sst>
 </file>
@@ -746,27 +749,27 @@
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5546875" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.54296875" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.5546875" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.5546875" customWidth="1"/>
-    <col min="17" max="17" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.54296875" customWidth="1"/>
+    <col min="11" max="11" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.54296875" customWidth="1"/>
+    <col min="13" max="13" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.54296875" customWidth="1"/>
+    <col min="17" max="17" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>13</v>
       </c>
@@ -792,7 +795,7 @@
       </c>
       <c r="Q4" s="8"/>
     </row>
-    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -830,7 +833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -868,7 +871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -906,7 +909,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -944,7 +947,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -970,7 +973,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -988,7 +991,7 @@
       </c>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1012,7 +1015,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
         <v>40</v>
       </c>
@@ -1026,7 +1029,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -1038,7 +1041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1056,7 +1059,7 @@
       </c>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J15" t="s">
         <v>25</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J16" t="s">
         <v>35</v>
       </c>
@@ -1072,7 +1075,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
     </row>
@@ -1092,23 +1095,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AI26"/>
+  <dimension ref="A1:AL26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AH16" sqref="AH16"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC19" sqref="AC19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.90625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="16" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -1187,28 +1190,34 @@
         <v>65</v>
       </c>
       <c r="AB1" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC1" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE1" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AC1" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE1" s="14" t="s">
+      <c r="AF1" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH1" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="AF1" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH1" s="14" t="s">
+      <c r="AI1" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK1" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="AI1" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AL1" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>88</v>
       </c>
@@ -1296,23 +1305,29 @@
       <c r="AC2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AD2" t="s">
-        <v>65</v>
-      </c>
       <c r="AE2" s="1" t="s">
         <v>88</v>
       </c>
       <c r="AF2" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="AG2" t="s">
+        <v>65</v>
+      </c>
       <c r="AH2" s="1" t="s">
         <v>88</v>
       </c>
       <c r="AI2" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AK2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1400,23 +1415,29 @@
       <c r="AC3" t="s">
         <v>68</v>
       </c>
-      <c r="AD3" t="s">
-        <v>65</v>
-      </c>
       <c r="AE3" t="s">
         <v>2</v>
       </c>
       <c r="AF3" t="s">
         <v>68</v>
       </c>
+      <c r="AG3" t="s">
+        <v>65</v>
+      </c>
       <c r="AH3" t="s">
         <v>2</v>
       </c>
       <c r="AI3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AK3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1499,19 +1520,19 @@
         <v>65</v>
       </c>
       <c r="AB4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE4" t="s">
         <v>62</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AF4" t="s">
         <v>76</v>
       </c>
-      <c r="AD4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>68</v>
+      <c r="AG4" t="s">
+        <v>65</v>
       </c>
       <c r="AH4" t="s">
         <v>55</v>
@@ -1519,8 +1540,14 @@
       <c r="AI4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AK4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1603,19 +1630,19 @@
         <v>65</v>
       </c>
       <c r="AB5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE5" t="s">
         <v>63</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AF5" t="s">
         <v>76</v>
       </c>
-      <c r="AD5" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>96</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>97</v>
+      <c r="AG5" t="s">
+        <v>65</v>
       </c>
       <c r="AH5" t="s">
         <v>96</v>
@@ -1623,8 +1650,14 @@
       <c r="AI5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AK5" t="s">
+        <v>96</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1707,28 +1740,34 @@
         <v>65</v>
       </c>
       <c r="AB6" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="AC6" t="s">
         <v>69</v>
       </c>
-      <c r="AD6" t="s">
-        <v>65</v>
-      </c>
       <c r="AE6" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AF6" t="s">
         <v>69</v>
       </c>
+      <c r="AG6" t="s">
+        <v>65</v>
+      </c>
       <c r="AH6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI6" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AK6" t="s">
+        <v>101</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1798,17 +1837,17 @@
       <c r="AA7" t="s">
         <v>65</v>
       </c>
-      <c r="AB7" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AE7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -1884,19 +1923,19 @@
       <c r="AA8" t="s">
         <v>65</v>
       </c>
-      <c r="AB8" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE8" s="7" t="s">
+      <c r="AB8" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="AF8" s="7" t="s">
+      <c r="AC8" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG8" t="s">
         <v>65</v>
       </c>
       <c r="AH8" s="7" t="s">
@@ -1905,8 +1944,14 @@
       <c r="AI8" s="7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="9" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AK8" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL8" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
         <v>87</v>
       </c>
@@ -1988,23 +2033,23 @@
       <c r="AA9" t="s">
         <v>65</v>
       </c>
-      <c r="AB9" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>65</v>
-      </c>
       <c r="AE9" t="s">
         <v>65</v>
       </c>
       <c r="AF9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AG9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2086,23 +2131,23 @@
       <c r="AA10" t="s">
         <v>65</v>
       </c>
-      <c r="AB10" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>65</v>
-      </c>
       <c r="AE10" t="s">
         <v>65</v>
       </c>
       <c r="AF10" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AG10" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -2178,23 +2223,23 @@
       <c r="AA11" t="s">
         <v>65</v>
       </c>
-      <c r="AB11" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>65</v>
-      </c>
       <c r="AE11" t="s">
         <v>65</v>
       </c>
       <c r="AF11" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AG11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -2270,23 +2315,23 @@
       <c r="AA12" t="s">
         <v>65</v>
       </c>
-      <c r="AB12" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>65</v>
-      </c>
       <c r="AE12" t="s">
         <v>65</v>
       </c>
       <c r="AF12" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="13" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AG12" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -2368,23 +2413,23 @@
       <c r="AA13" t="s">
         <v>65</v>
       </c>
-      <c r="AB13" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>65</v>
-      </c>
       <c r="AE13" t="s">
         <v>65</v>
       </c>
       <c r="AF13" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AG13" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -2466,23 +2511,23 @@
       <c r="AA14" t="s">
         <v>65</v>
       </c>
-      <c r="AB14" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>65</v>
-      </c>
       <c r="AE14" t="s">
         <v>65</v>
       </c>
       <c r="AF14" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AG14" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -2558,23 +2603,23 @@
       <c r="AA15" t="s">
         <v>65</v>
       </c>
-      <c r="AB15" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>65</v>
-      </c>
       <c r="AE15" t="s">
         <v>65</v>
       </c>
       <c r="AF15" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="16" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AG15" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -2656,23 +2701,23 @@
       <c r="AA16" t="s">
         <v>65</v>
       </c>
-      <c r="AB16" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC16" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD16" t="s">
-        <v>65</v>
-      </c>
       <c r="AE16" t="s">
         <v>65</v>
       </c>
       <c r="AF16" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG16" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -2754,23 +2799,23 @@
       <c r="AA17" t="s">
         <v>65</v>
       </c>
-      <c r="AB17" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>65</v>
-      </c>
       <c r="AE17" t="s">
         <v>65</v>
       </c>
       <c r="AF17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -2852,23 +2897,23 @@
       <c r="AA18" t="s">
         <v>65</v>
       </c>
-      <c r="AB18" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>65</v>
-      </c>
       <c r="AE18" t="s">
         <v>65</v>
       </c>
       <c r="AF18" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG18" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -2950,23 +2995,23 @@
       <c r="AA19" t="s">
         <v>65</v>
       </c>
-      <c r="AB19" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC19" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD19" t="s">
-        <v>65</v>
-      </c>
       <c r="AE19" t="s">
         <v>65</v>
       </c>
       <c r="AF19" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -3042,23 +3087,23 @@
       <c r="AA20" t="s">
         <v>65</v>
       </c>
-      <c r="AB20" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC20" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD20" t="s">
-        <v>65</v>
-      </c>
       <c r="AE20" t="s">
         <v>65</v>
       </c>
       <c r="AF20" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG20" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -3134,23 +3179,23 @@
       <c r="AA21" t="s">
         <v>65</v>
       </c>
-      <c r="AB21" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC21" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD21" t="s">
-        <v>65</v>
-      </c>
       <c r="AE21" t="s">
         <v>65</v>
       </c>
       <c r="AF21" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG21" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -3226,23 +3271,23 @@
       <c r="AA22" t="s">
         <v>65</v>
       </c>
-      <c r="AB22" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC22" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD22" t="s">
-        <v>65</v>
-      </c>
       <c r="AE22" t="s">
         <v>65</v>
       </c>
       <c r="AF22" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG22" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -3318,23 +3363,23 @@
       <c r="AA23" t="s">
         <v>65</v>
       </c>
-      <c r="AB23" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC23" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD23" t="s">
-        <v>65</v>
-      </c>
       <c r="AE23" t="s">
         <v>65</v>
       </c>
       <c r="AF23" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG23" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -3410,23 +3455,23 @@
       <c r="AA24" t="s">
         <v>65</v>
       </c>
-      <c r="AB24" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC24" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD24" t="s">
-        <v>65</v>
-      </c>
       <c r="AE24" t="s">
         <v>65</v>
       </c>
       <c r="AF24" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AG24" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH24" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
       <c r="G25" t="s">
         <v>83</v>
       </c>
@@ -3434,7 +3479,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
       <c r="G26" t="s">
         <v>98</v>
       </c>
@@ -3443,19 +3488,20 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="AK1:AL1"/>
     <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AB1:AC1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>